<commit_message>
added track_number and rake_id in Rake
</commit_message>
<xml_diff>
--- a/rake_data/gt_inward_summary.xlsx
+++ b/rake_data/gt_inward_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t xml:space="preserve">train_number</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">train_destination_station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">track_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rake_id</t>
   </si>
   <si>
     <t xml:space="preserve">rake_type</t>
@@ -174,7 +180,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -195,11 +201,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -257,7 +258,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,10 +279,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -289,38 +290,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="10.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="19.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="34" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="19.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,22 +347,22 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="0" t="s">
@@ -396,13 +398,13 @@
       <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -411,85 +413,91 @@
       <c r="AC1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="0" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="AI1" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>63251201909</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="0" t="s">
+      <c r="N2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>41</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="V2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE2" s="0" t="s">
+      <c r="Z2" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="AA2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="AG2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>